<commit_message>
create: NaiveBayesV3 Model && Controller && setupDatasetTable
</commit_message>
<xml_diff>
--- a/hitung_manual.xlsx
+++ b/hitung_manual.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="70">
   <si>
     <t>NO.</t>
   </si>
@@ -169,10 +169,7 @@
     <t>70 - 74,9 = B-</t>
   </si>
   <si>
-    <t>55 - 70 = C</t>
-  </si>
-  <si>
-    <t>0 - 54,9 = D/E</t>
+    <t>0 - 70 = C/D/E</t>
   </si>
   <si>
     <t>Jurusan:</t>
@@ -205,10 +202,10 @@
     <t>A</t>
   </si>
   <si>
+    <t>C/D/E</t>
+  </si>
+  <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>D/E</t>
   </si>
   <si>
     <t>P(NO)</t>
@@ -3378,7 +3375,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:P2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -3783,9 +3780,7 @@
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="23" t="s">
-        <v>51</v>
-      </c>
+      <c r="A15" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3796,10 +3791,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BZ22"/>
+  <dimension ref="A1:BZ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -3822,13 +3817,14 @@
     <col min="55" max="55" width="19.0095238095238" customWidth="1"/>
     <col min="60" max="60" width="17.2666666666667" customWidth="1"/>
     <col min="65" max="65" width="17.0095238095238" customWidth="1"/>
+    <col min="70" max="70" width="12.8571428571429"/>
     <col min="75" max="75" width="14.7714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1"/>
     <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>'2. MEAN TO DISCREATE'!R2</f>
@@ -3853,337 +3849,337 @@
         <v>7</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R3" s="7"/>
       <c r="S3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="W3" s="7"/>
       <c r="X3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Z3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AB3" s="7"/>
       <c r="AC3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AE3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="AF3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG3" s="7"/>
       <c r="AH3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AJ3" s="5" t="s">
         <v>14</v>
       </c>
       <c r="AK3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AL3" s="7"/>
       <c r="AM3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AO3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="AP3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AQ3" s="7"/>
       <c r="AR3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AT3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="AU3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AV3" s="7"/>
       <c r="AW3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AY3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="AZ3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BA3" s="7"/>
       <c r="BB3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BD3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="BE3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BF3" s="7"/>
       <c r="BG3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BI3" s="5" t="s">
         <v>18</v>
       </c>
       <c r="BJ3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BK3" s="7"/>
       <c r="BL3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BN3" s="5" t="s">
         <v>19</v>
       </c>
       <c r="BO3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BP3" s="7"/>
       <c r="BQ3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BS3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="BT3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BU3" s="7"/>
       <c r="BV3" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BX3" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="BY3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BZ3" s="7"/>
     </row>
     <row r="4" ht="77" customHeight="1" spans="1:78">
       <c r="A4" s="5"/>
       <c r="B4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="N4" s="10"/>
       <c r="O4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P4" s="5"/>
       <c r="Q4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="R4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="S4" s="10"/>
       <c r="T4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U4" s="5"/>
       <c r="V4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="W4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="W4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="X4" s="10"/>
       <c r="Y4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z4" s="5"/>
       <c r="AA4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="AB4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="AC4" s="10"/>
       <c r="AD4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AE4" s="5"/>
       <c r="AF4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="AG4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="AH4" s="10"/>
       <c r="AI4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AJ4" s="5"/>
       <c r="AK4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="AL4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="AM4" s="10"/>
       <c r="AN4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AO4" s="5"/>
       <c r="AP4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="AQ4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="AR4" s="10"/>
       <c r="AS4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AT4" s="5"/>
       <c r="AU4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AV4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="AV4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="AW4" s="10"/>
       <c r="AX4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AY4" s="5"/>
       <c r="AZ4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="BA4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="BA4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="BB4" s="10"/>
       <c r="BC4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BD4" s="5"/>
       <c r="BE4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="BF4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="BF4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="BG4" s="10"/>
       <c r="BH4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BI4" s="5"/>
       <c r="BJ4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="BK4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="BK4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="BL4" s="10"/>
       <c r="BM4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BN4" s="5"/>
       <c r="BO4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="BP4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="BP4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="BQ4" s="10"/>
       <c r="BR4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BS4" s="5"/>
       <c r="BT4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="BU4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="BU4" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="BV4" s="10"/>
       <c r="BW4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BX4" s="5"/>
       <c r="BY4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="BZ4" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="BZ4" s="9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:78">
       <c r="A5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="13">
         <v>1</v>
@@ -4192,15 +4188,15 @@
         <v>1</v>
       </c>
       <c r="D5" s="14">
-        <f>SUM(B5:C5)</f>
+        <f t="shared" ref="D5:D10" si="0">SUM(B5:C5)</f>
         <v>2</v>
       </c>
       <c r="E5" s="15">
-        <f>D5/D$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="E5:E12" si="1">D5/D$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G5" s="13">
         <v>1</v>
@@ -4209,15 +4205,15 @@
         <v>1</v>
       </c>
       <c r="I5" s="14">
-        <f>SUM(G5:H5)</f>
+        <f t="shared" ref="I5:I10" si="2">SUM(G5:H5)</f>
         <v>2</v>
       </c>
       <c r="J5" s="15">
-        <f t="shared" ref="J5:J12" si="0">I5/I$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="J5:J12" si="3">I5/I$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L5" s="13">
         <v>1</v>
@@ -4226,15 +4222,15 @@
         <v>1</v>
       </c>
       <c r="N5" s="14">
-        <f>SUM(L5:M5)</f>
+        <f t="shared" ref="N5:N10" si="4">SUM(L5:M5)</f>
         <v>2</v>
       </c>
       <c r="O5" s="15">
-        <f t="shared" ref="O5:O12" si="1">N5/N$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="O5:O12" si="5">N5/N$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q5" s="13">
         <v>1</v>
@@ -4243,15 +4239,15 @@
         <v>1</v>
       </c>
       <c r="S5" s="14">
-        <f>SUM(Q5:R5)</f>
+        <f t="shared" ref="S5:S10" si="6">SUM(Q5:R5)</f>
         <v>2</v>
       </c>
       <c r="T5" s="15">
-        <f t="shared" ref="T5:T12" si="2">S5/S$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="T5:T12" si="7">S5/S$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V5" s="13">
         <v>1</v>
@@ -4260,15 +4256,15 @@
         <v>1</v>
       </c>
       <c r="X5" s="14">
-        <f>SUM(V5:W5)</f>
+        <f t="shared" ref="X5:X10" si="8">SUM(V5:W5)</f>
         <v>2</v>
       </c>
       <c r="Y5" s="15">
-        <f t="shared" ref="Y5:Y12" si="3">X5/X$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="Y5:Y12" si="9">X5/X$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="Z5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AA5" s="13">
         <v>1</v>
@@ -4277,15 +4273,15 @@
         <v>1</v>
       </c>
       <c r="AC5" s="14">
-        <f>SUM(AA5:AB5)</f>
+        <f t="shared" ref="AC5:AC10" si="10">SUM(AA5:AB5)</f>
         <v>2</v>
       </c>
       <c r="AD5" s="15">
-        <f t="shared" ref="AD5:AD12" si="4">AC5/AC$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="AD5:AD12" si="11">AC5/AC$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="AE5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AF5" s="13">
         <v>1</v>
@@ -4294,15 +4290,15 @@
         <v>1</v>
       </c>
       <c r="AH5" s="14">
-        <f>SUM(AF5:AG5)</f>
+        <f t="shared" ref="AH5:AH10" si="12">SUM(AF5:AG5)</f>
         <v>2</v>
       </c>
       <c r="AI5" s="15">
-        <f t="shared" ref="AI5:AI12" si="5">AH5/AH$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="AI5:AI12" si="13">AH5/AH$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="AJ5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AK5" s="13">
         <v>1</v>
@@ -4311,15 +4307,15 @@
         <v>1</v>
       </c>
       <c r="AM5" s="14">
-        <f>SUM(AK5:AL5)</f>
+        <f t="shared" ref="AM5:AM10" si="14">SUM(AK5:AL5)</f>
         <v>2</v>
       </c>
       <c r="AN5" s="15">
-        <f t="shared" ref="AN5:AN12" si="6">AM5/AM$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="AN5:AN12" si="15">AM5/AM$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="AO5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AP5" s="13">
         <v>1</v>
@@ -4328,15 +4324,15 @@
         <v>1</v>
       </c>
       <c r="AR5" s="14">
-        <f>SUM(AP5:AQ5)</f>
+        <f t="shared" ref="AR5:AR10" si="16">SUM(AP5:AQ5)</f>
         <v>2</v>
       </c>
       <c r="AS5" s="15">
-        <f t="shared" ref="AS5:AS12" si="7">AR5/AR$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="AS5:AS12" si="17">AR5/AR$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="AT5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AU5" s="13">
         <v>1</v>
@@ -4345,15 +4341,15 @@
         <v>1</v>
       </c>
       <c r="AW5" s="14">
-        <f>SUM(AU5:AV5)</f>
+        <f t="shared" ref="AW5:AW10" si="18">SUM(AU5:AV5)</f>
         <v>2</v>
       </c>
       <c r="AX5" s="15">
-        <f t="shared" ref="AX5:AX12" si="8">AW5/AW$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="AX5:AX12" si="19">AW5/AW$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="AY5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AZ5" s="13">
         <v>1</v>
@@ -4362,15 +4358,15 @@
         <v>1</v>
       </c>
       <c r="BB5" s="14">
-        <f>SUM(AZ5:BA5)</f>
+        <f t="shared" ref="BB5:BB10" si="20">SUM(AZ5:BA5)</f>
         <v>2</v>
       </c>
       <c r="BC5" s="15">
-        <f t="shared" ref="BC5:BC12" si="9">BB5/BB$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="BC5:BC12" si="21">BB5/BB$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="BD5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BE5" s="13">
         <v>1</v>
@@ -4379,15 +4375,15 @@
         <v>1</v>
       </c>
       <c r="BG5" s="14">
-        <f>SUM(BE5:BF5)</f>
+        <f t="shared" ref="BG5:BG10" si="22">SUM(BE5:BF5)</f>
         <v>2</v>
       </c>
       <c r="BH5" s="15">
-        <f t="shared" ref="BH5:BH12" si="10">BG5/BG$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="BH5:BH12" si="23">BG5/BG$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="BI5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BJ5" s="13">
         <v>1</v>
@@ -4396,15 +4392,15 @@
         <v>1</v>
       </c>
       <c r="BL5" s="14">
-        <f>SUM(BJ5:BK5)</f>
+        <f t="shared" ref="BL5:BL10" si="24">SUM(BJ5:BK5)</f>
         <v>2</v>
       </c>
       <c r="BM5" s="15">
-        <f t="shared" ref="BM5:BM12" si="11">BL5/BL$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="BM5:BM12" si="25">BL5/BL$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="BN5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BO5" s="13">
         <v>1</v>
@@ -4413,15 +4409,15 @@
         <v>1</v>
       </c>
       <c r="BQ5" s="14">
-        <f>SUM(BO5:BP5)</f>
+        <f t="shared" ref="BQ5:BQ10" si="26">SUM(BO5:BP5)</f>
         <v>2</v>
       </c>
       <c r="BR5" s="15">
-        <f t="shared" ref="BR5:BR12" si="12">BQ5/BQ$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="BR5:BR12" si="27">BQ5/BQ$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="BS5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BT5" s="13">
         <v>1</v>
@@ -4430,12 +4426,12 @@
         <v>1</v>
       </c>
       <c r="BV5" s="14">
-        <f>SUM(BT5:BU5)</f>
+        <f t="shared" ref="BV5:BV10" si="28">SUM(BT5:BU5)</f>
         <v>2</v>
       </c>
       <c r="BW5" s="15">
-        <f t="shared" ref="BW5:BW12" si="13">BV5/BV$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" ref="BW5:BW12" si="29">BV5/BV$11</f>
+        <v>0.153846153846154</v>
       </c>
       <c r="BX5" s="12"/>
       <c r="BY5" s="13">
@@ -4456,12 +4452,12 @@
         <v>2</v>
       </c>
       <c r="D6" s="14">
-        <f t="shared" ref="D6:D11" si="14">SUM(B6:C6)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E6" s="15">
-        <f>D6/D$12</f>
-        <v>0.2</v>
+        <f t="shared" si="1"/>
+        <v>0.230769230769231</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>40</v>
@@ -4473,12 +4469,12 @@
         <v>2</v>
       </c>
       <c r="I6" s="14">
-        <f t="shared" ref="I6:I11" si="15">SUM(G6:H6)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J6" s="15">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
+        <f t="shared" si="3"/>
+        <v>0.230769230769231</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>40</v>
@@ -4490,12 +4486,12 @@
         <v>1</v>
       </c>
       <c r="N6" s="14">
-        <f t="shared" ref="N6:N11" si="16">SUM(L6:M6)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="O6" s="15">
-        <f t="shared" si="1"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="5"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="P6" s="12" t="s">
         <v>40</v>
@@ -4507,12 +4503,12 @@
         <v>1</v>
       </c>
       <c r="S6" s="14">
-        <f t="shared" ref="S6:S11" si="17">SUM(Q6:R6)</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="T6" s="15">
-        <f t="shared" si="2"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="7"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="U6" s="12" t="s">
         <v>40</v>
@@ -4524,12 +4520,12 @@
         <v>1</v>
       </c>
       <c r="X6" s="14">
-        <f t="shared" ref="X6:X11" si="18">SUM(V6:W6)</f>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="Y6" s="15">
-        <f t="shared" si="3"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="9"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="Z6" s="12" t="s">
         <v>40</v>
@@ -4541,12 +4537,12 @@
         <v>1</v>
       </c>
       <c r="AC6" s="14">
-        <f t="shared" ref="AC6:AC11" si="19">SUM(AA6:AB6)</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="AD6" s="15">
-        <f t="shared" si="4"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="11"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AE6" s="12" t="s">
         <v>40</v>
@@ -4558,12 +4554,12 @@
         <v>1</v>
       </c>
       <c r="AH6" s="14">
-        <f t="shared" ref="AH6:AH11" si="20">SUM(AF6:AG6)</f>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="AI6" s="15">
-        <f t="shared" si="5"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="13"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AJ6" s="12" t="s">
         <v>40</v>
@@ -4575,12 +4571,12 @@
         <v>1</v>
       </c>
       <c r="AM6" s="14">
-        <f t="shared" ref="AM6:AM11" si="21">SUM(AK6:AL6)</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="AN6" s="15">
-        <f t="shared" si="6"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="15"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AO6" s="12" t="s">
         <v>40</v>
@@ -4592,12 +4588,12 @@
         <v>1</v>
       </c>
       <c r="AR6" s="14">
-        <f t="shared" ref="AR6:AR11" si="22">SUM(AP6:AQ6)</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AS6" s="15">
-        <f t="shared" si="7"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="17"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AT6" s="12" t="s">
         <v>40</v>
@@ -4609,12 +4605,12 @@
         <v>1</v>
       </c>
       <c r="AW6" s="14">
-        <f t="shared" ref="AW6:AW11" si="23">SUM(AU6:AV6)</f>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="AX6" s="15">
-        <f t="shared" si="8"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="19"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AY6" s="12" t="s">
         <v>40</v>
@@ -4626,12 +4622,12 @@
         <v>1</v>
       </c>
       <c r="BB6" s="14">
-        <f t="shared" ref="BB6:BB11" si="24">SUM(AZ6:BA6)</f>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="BC6" s="15">
-        <f t="shared" si="9"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="21"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BD6" s="12" t="s">
         <v>40</v>
@@ -4643,12 +4639,12 @@
         <v>1</v>
       </c>
       <c r="BG6" s="14">
-        <f t="shared" ref="BG6:BG11" si="25">SUM(BE6:BF6)</f>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="BH6" s="15">
-        <f t="shared" si="10"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="23"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BI6" s="12" t="s">
         <v>40</v>
@@ -4660,12 +4656,12 @@
         <v>1</v>
       </c>
       <c r="BL6" s="14">
-        <f t="shared" ref="BL6:BL11" si="26">SUM(BJ6:BK6)</f>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
       <c r="BM6" s="15">
-        <f t="shared" si="11"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="25"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BN6" s="12" t="s">
         <v>40</v>
@@ -4677,12 +4673,12 @@
         <v>1</v>
       </c>
       <c r="BQ6" s="14">
-        <f t="shared" ref="BQ6:BQ11" si="27">SUM(BO6:BP6)</f>
+        <f t="shared" si="26"/>
         <v>2</v>
       </c>
       <c r="BR6" s="15">
-        <f t="shared" si="12"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="27"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BS6" s="12" t="s">
         <v>40</v>
@@ -4694,12 +4690,12 @@
         <v>1</v>
       </c>
       <c r="BV6" s="14">
-        <f t="shared" ref="BV6:BV11" si="28">SUM(BT6:BU6)</f>
+        <f t="shared" si="28"/>
         <v>2</v>
       </c>
       <c r="BW6" s="15">
-        <f t="shared" si="13"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="29"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BX6" s="12"/>
       <c r="BY6" s="13">
@@ -4720,12 +4716,12 @@
         <v>1</v>
       </c>
       <c r="D7" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E7" s="15">
-        <f>D7/D$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" si="1"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>41</v>
@@ -4737,12 +4733,12 @@
         <v>1</v>
       </c>
       <c r="I7" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J7" s="15">
-        <f t="shared" si="0"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="3"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>41</v>
@@ -4754,148 +4750,148 @@
         <v>2</v>
       </c>
       <c r="N7" s="14">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="O7" s="15">
+        <f t="shared" si="5"/>
+        <v>0.230769230769231</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q7" s="13">
+        <v>1</v>
+      </c>
+      <c r="R7" s="13">
+        <v>1</v>
+      </c>
+      <c r="S7" s="14">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="T7" s="15">
+        <f t="shared" si="7"/>
+        <v>0.153846153846154</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="V7" s="13">
+        <v>1</v>
+      </c>
+      <c r="W7" s="13">
+        <v>2</v>
+      </c>
+      <c r="X7" s="14">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="Y7" s="15">
+        <f t="shared" si="9"/>
+        <v>0.230769230769231</v>
+      </c>
+      <c r="Z7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA7" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="13">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="14">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="AD7" s="15">
+        <f t="shared" si="11"/>
+        <v>0.230769230769231</v>
+      </c>
+      <c r="AE7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF7" s="13">
+        <v>1</v>
+      </c>
+      <c r="AG7" s="13">
+        <v>2</v>
+      </c>
+      <c r="AH7" s="14">
+        <f t="shared" si="12"/>
+        <v>3</v>
+      </c>
+      <c r="AI7" s="15">
+        <f t="shared" si="13"/>
+        <v>0.230769230769231</v>
+      </c>
+      <c r="AJ7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK7" s="13">
+        <v>1</v>
+      </c>
+      <c r="AL7" s="13">
+        <v>2</v>
+      </c>
+      <c r="AM7" s="14">
+        <f t="shared" si="14"/>
+        <v>3</v>
+      </c>
+      <c r="AN7" s="15">
+        <f t="shared" si="15"/>
+        <v>0.230769230769231</v>
+      </c>
+      <c r="AO7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP7" s="13">
+        <v>1</v>
+      </c>
+      <c r="AQ7" s="13">
+        <v>2</v>
+      </c>
+      <c r="AR7" s="14">
         <f t="shared" si="16"/>
         <v>3</v>
       </c>
-      <c r="O7" s="15">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="P7" s="12" t="s">
+      <c r="AS7" s="15">
+        <f t="shared" si="17"/>
+        <v>0.230769230769231</v>
+      </c>
+      <c r="AT7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="Q7" s="13">
-        <v>1</v>
-      </c>
-      <c r="R7" s="13">
-        <v>1</v>
-      </c>
-      <c r="S7" s="14">
-        <f t="shared" si="17"/>
-        <v>2</v>
-      </c>
-      <c r="T7" s="15">
-        <f t="shared" si="2"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="U7" s="12" t="s">
+      <c r="AU7" s="13">
+        <v>1</v>
+      </c>
+      <c r="AV7" s="13">
+        <v>1</v>
+      </c>
+      <c r="AW7" s="14">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="AX7" s="15">
+        <f t="shared" si="19"/>
+        <v>0.153846153846154</v>
+      </c>
+      <c r="AY7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="V7" s="13">
-        <v>1</v>
-      </c>
-      <c r="W7" s="13">
-        <v>2</v>
-      </c>
-      <c r="X7" s="14">
-        <f t="shared" si="18"/>
-        <v>3</v>
-      </c>
-      <c r="Y7" s="15">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="Z7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA7" s="13">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="13">
-        <v>2</v>
-      </c>
-      <c r="AC7" s="14">
-        <f t="shared" si="19"/>
-        <v>3</v>
-      </c>
-      <c r="AD7" s="15">
-        <f t="shared" si="4"/>
-        <v>0.2</v>
-      </c>
-      <c r="AE7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF7" s="13">
-        <v>1</v>
-      </c>
-      <c r="AG7" s="13">
-        <v>2</v>
-      </c>
-      <c r="AH7" s="14">
+      <c r="AZ7" s="13">
+        <v>1</v>
+      </c>
+      <c r="BA7" s="13">
+        <v>2</v>
+      </c>
+      <c r="BB7" s="14">
         <f t="shared" si="20"/>
         <v>3</v>
       </c>
-      <c r="AI7" s="15">
-        <f t="shared" si="5"/>
-        <v>0.2</v>
-      </c>
-      <c r="AJ7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AK7" s="13">
-        <v>1</v>
-      </c>
-      <c r="AL7" s="13">
-        <v>2</v>
-      </c>
-      <c r="AM7" s="14">
+      <c r="BC7" s="15">
         <f t="shared" si="21"/>
-        <v>3</v>
-      </c>
-      <c r="AN7" s="15">
-        <f t="shared" si="6"/>
-        <v>0.2</v>
-      </c>
-      <c r="AO7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AP7" s="13">
-        <v>1</v>
-      </c>
-      <c r="AQ7" s="13">
-        <v>2</v>
-      </c>
-      <c r="AR7" s="14">
-        <f t="shared" si="22"/>
-        <v>3</v>
-      </c>
-      <c r="AS7" s="15">
-        <f t="shared" si="7"/>
-        <v>0.2</v>
-      </c>
-      <c r="AT7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU7" s="13">
-        <v>1</v>
-      </c>
-      <c r="AV7" s="13">
-        <v>1</v>
-      </c>
-      <c r="AW7" s="14">
-        <f t="shared" si="23"/>
-        <v>2</v>
-      </c>
-      <c r="AX7" s="15">
-        <f t="shared" si="8"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="AY7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AZ7" s="13">
-        <v>1</v>
-      </c>
-      <c r="BA7" s="13">
-        <v>2</v>
-      </c>
-      <c r="BB7" s="14">
-        <f t="shared" si="24"/>
-        <v>3</v>
-      </c>
-      <c r="BC7" s="15">
-        <f t="shared" si="9"/>
-        <v>0.2</v>
+        <v>0.230769230769231</v>
       </c>
       <c r="BD7" s="12" t="s">
         <v>41</v>
@@ -4907,12 +4903,12 @@
         <v>1</v>
       </c>
       <c r="BG7" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="BH7" s="15">
-        <f t="shared" si="10"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="23"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BI7" s="12" t="s">
         <v>41</v>
@@ -4924,12 +4920,12 @@
         <v>1</v>
       </c>
       <c r="BL7" s="14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
       <c r="BM7" s="15">
-        <f t="shared" si="11"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="25"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BN7" s="12" t="s">
         <v>41</v>
@@ -4941,12 +4937,12 @@
         <v>1</v>
       </c>
       <c r="BQ7" s="14">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="BR7" s="15">
         <f t="shared" si="27"/>
-        <v>2</v>
-      </c>
-      <c r="BR7" s="15">
-        <f t="shared" si="12"/>
-        <v>0.133333333333333</v>
+        <v>0.153846153846154</v>
       </c>
       <c r="BS7" s="12" t="s">
         <v>41</v>
@@ -4962,8 +4958,8 @@
         <v>2</v>
       </c>
       <c r="BW7" s="15">
-        <f t="shared" si="13"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="29"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BX7" s="12"/>
       <c r="BY7" s="13">
@@ -4984,12 +4980,12 @@
         <v>1</v>
       </c>
       <c r="D8" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E8" s="15">
-        <f>D8/D$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" si="1"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>42</v>
@@ -5001,12 +4997,12 @@
         <v>1</v>
       </c>
       <c r="I8" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J8" s="15">
-        <f t="shared" si="0"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="3"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>42</v>
@@ -5018,12 +5014,12 @@
         <v>1</v>
       </c>
       <c r="N8" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="O8" s="15">
-        <f t="shared" si="1"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="5"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="P8" s="12" t="s">
         <v>42</v>
@@ -5035,12 +5031,12 @@
         <v>2</v>
       </c>
       <c r="S8" s="14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="T8" s="15">
-        <f t="shared" si="2"/>
-        <v>0.2</v>
+        <f t="shared" si="7"/>
+        <v>0.230769230769231</v>
       </c>
       <c r="U8" s="12" t="s">
         <v>42</v>
@@ -5052,12 +5048,12 @@
         <v>1</v>
       </c>
       <c r="X8" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="Y8" s="15">
-        <f t="shared" si="3"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="9"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="Z8" s="12" t="s">
         <v>42</v>
@@ -5069,12 +5065,12 @@
         <v>1</v>
       </c>
       <c r="AC8" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="AD8" s="15">
-        <f t="shared" si="4"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="11"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AE8" s="12" t="s">
         <v>42</v>
@@ -5086,12 +5082,12 @@
         <v>1</v>
       </c>
       <c r="AH8" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="AI8" s="15">
-        <f t="shared" si="5"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="13"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AJ8" s="12" t="s">
         <v>42</v>
@@ -5103,12 +5099,12 @@
         <v>1</v>
       </c>
       <c r="AM8" s="14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="AN8" s="15">
-        <f t="shared" si="6"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="15"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AO8" s="12" t="s">
         <v>42</v>
@@ -5120,12 +5116,12 @@
         <v>1</v>
       </c>
       <c r="AR8" s="14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AS8" s="15">
-        <f t="shared" si="7"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="17"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AT8" s="12" t="s">
         <v>42</v>
@@ -5137,12 +5133,12 @@
         <v>2</v>
       </c>
       <c r="AW8" s="14">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="AX8" s="15">
-        <f t="shared" si="8"/>
-        <v>0.2</v>
+        <f t="shared" si="19"/>
+        <v>0.230769230769231</v>
       </c>
       <c r="AY8" s="12" t="s">
         <v>42</v>
@@ -5154,12 +5150,12 @@
         <v>1</v>
       </c>
       <c r="BB8" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="BC8" s="15">
-        <f t="shared" si="9"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="21"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BD8" s="12" t="s">
         <v>42</v>
@@ -5171,12 +5167,12 @@
         <v>2</v>
       </c>
       <c r="BG8" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>3</v>
       </c>
       <c r="BH8" s="15">
-        <f t="shared" si="10"/>
-        <v>0.2</v>
+        <f t="shared" si="23"/>
+        <v>0.230769230769231</v>
       </c>
       <c r="BI8" s="12" t="s">
         <v>42</v>
@@ -5188,29 +5184,29 @@
         <v>2</v>
       </c>
       <c r="BL8" s="14">
+        <f t="shared" si="24"/>
+        <v>3</v>
+      </c>
+      <c r="BM8" s="15">
+        <f t="shared" si="25"/>
+        <v>0.230769230769231</v>
+      </c>
+      <c r="BN8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="BO8" s="13">
+        <v>1</v>
+      </c>
+      <c r="BP8" s="13">
+        <v>2</v>
+      </c>
+      <c r="BQ8" s="14">
         <f t="shared" si="26"/>
         <v>3</v>
       </c>
-      <c r="BM8" s="15">
-        <f t="shared" si="11"/>
-        <v>0.2</v>
-      </c>
-      <c r="BN8" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="BO8" s="13">
-        <v>1</v>
-      </c>
-      <c r="BP8" s="13">
-        <v>2</v>
-      </c>
-      <c r="BQ8" s="14">
+      <c r="BR8" s="15">
         <f t="shared" si="27"/>
-        <v>3</v>
-      </c>
-      <c r="BR8" s="15">
-        <f t="shared" si="12"/>
-        <v>0.2</v>
+        <v>0.230769230769231</v>
       </c>
       <c r="BS8" s="12" t="s">
         <v>42</v>
@@ -5226,8 +5222,8 @@
         <v>3</v>
       </c>
       <c r="BW8" s="15">
-        <f t="shared" si="13"/>
-        <v>0.2</v>
+        <f t="shared" si="29"/>
+        <v>0.230769230769231</v>
       </c>
       <c r="BX8" s="12"/>
       <c r="BY8" s="13">
@@ -5248,12 +5244,12 @@
         <v>1</v>
       </c>
       <c r="D9" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E9" s="15">
-        <f>D9/D$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" si="1"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>43</v>
@@ -5265,12 +5261,12 @@
         <v>1</v>
       </c>
       <c r="I9" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J9" s="15">
-        <f t="shared" si="0"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="3"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="K9" s="13" t="s">
         <v>43</v>
@@ -5282,12 +5278,12 @@
         <v>1</v>
       </c>
       <c r="N9" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="O9" s="15">
-        <f t="shared" si="1"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="5"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="P9" s="13" t="s">
         <v>43</v>
@@ -5299,12 +5295,12 @@
         <v>1</v>
       </c>
       <c r="S9" s="14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="T9" s="15">
-        <f t="shared" si="2"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="7"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="U9" s="13" t="s">
         <v>43</v>
@@ -5316,12 +5312,12 @@
         <v>1</v>
       </c>
       <c r="X9" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="Y9" s="15">
-        <f t="shared" si="3"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="9"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="Z9" s="13" t="s">
         <v>43</v>
@@ -5333,12 +5329,12 @@
         <v>1</v>
       </c>
       <c r="AC9" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="AD9" s="15">
-        <f t="shared" si="4"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="11"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AE9" s="13" t="s">
         <v>43</v>
@@ -5350,12 +5346,12 @@
         <v>1</v>
       </c>
       <c r="AH9" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="AI9" s="15">
-        <f t="shared" si="5"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="13"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AJ9" s="13" t="s">
         <v>43</v>
@@ -5367,12 +5363,12 @@
         <v>1</v>
       </c>
       <c r="AM9" s="14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="AN9" s="15">
-        <f t="shared" si="6"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="15"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AO9" s="13" t="s">
         <v>43</v>
@@ -5384,12 +5380,12 @@
         <v>1</v>
       </c>
       <c r="AR9" s="14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AS9" s="15">
-        <f t="shared" si="7"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="17"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AT9" s="13" t="s">
         <v>43</v>
@@ -5401,12 +5397,12 @@
         <v>1</v>
       </c>
       <c r="AW9" s="14">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="AX9" s="15">
-        <f t="shared" si="8"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="19"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AY9" s="13" t="s">
         <v>43</v>
@@ -5418,12 +5414,12 @@
         <v>1</v>
       </c>
       <c r="BB9" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="BC9" s="15">
-        <f t="shared" si="9"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="21"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BD9" s="13" t="s">
         <v>43</v>
@@ -5435,12 +5431,12 @@
         <v>1</v>
       </c>
       <c r="BG9" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="BH9" s="15">
-        <f t="shared" si="10"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="23"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BI9" s="13" t="s">
         <v>43</v>
@@ -5452,12 +5448,12 @@
         <v>1</v>
       </c>
       <c r="BL9" s="14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
       <c r="BM9" s="15">
-        <f t="shared" si="11"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="25"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BN9" s="13" t="s">
         <v>43</v>
@@ -5469,12 +5465,12 @@
         <v>1</v>
       </c>
       <c r="BQ9" s="14">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="BR9" s="15">
         <f t="shared" si="27"/>
-        <v>2</v>
-      </c>
-      <c r="BR9" s="15">
-        <f t="shared" si="12"/>
-        <v>0.133333333333333</v>
+        <v>0.153846153846154</v>
       </c>
       <c r="BS9" s="13" t="s">
         <v>43</v>
@@ -5490,8 +5486,8 @@
         <v>2</v>
       </c>
       <c r="BW9" s="15">
-        <f t="shared" si="13"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="29"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BX9" s="13"/>
       <c r="BY9" s="13">
@@ -5503,7 +5499,7 @@
     </row>
     <row r="10" spans="1:78">
       <c r="A10" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
@@ -5512,12 +5508,12 @@
         <v>1</v>
       </c>
       <c r="D10" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E10" s="15">
-        <f>D10/D$12</f>
-        <v>0.133333333333333</v>
+        <f t="shared" si="1"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>62</v>
@@ -5529,12 +5525,12 @@
         <v>1</v>
       </c>
       <c r="I10" s="14">
-        <f t="shared" si="15"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J10" s="15">
-        <f t="shared" si="0"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="3"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="K10" s="13" t="s">
         <v>62</v>
@@ -5546,12 +5542,12 @@
         <v>1</v>
       </c>
       <c r="N10" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="O10" s="15">
-        <f t="shared" si="1"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="5"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="P10" s="13" t="s">
         <v>62</v>
@@ -5563,12 +5559,12 @@
         <v>1</v>
       </c>
       <c r="S10" s="14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="T10" s="15">
-        <f t="shared" si="2"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="7"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="U10" s="13" t="s">
         <v>62</v>
@@ -5580,12 +5576,12 @@
         <v>1</v>
       </c>
       <c r="X10" s="14">
-        <f t="shared" si="18"/>
+        <f t="shared" si="8"/>
         <v>2</v>
       </c>
       <c r="Y10" s="15">
-        <f t="shared" si="3"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="9"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="Z10" s="13" t="s">
         <v>62</v>
@@ -5597,12 +5593,12 @@
         <v>1</v>
       </c>
       <c r="AC10" s="14">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="AD10" s="15">
-        <f t="shared" si="4"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="11"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AE10" s="13" t="s">
         <v>62</v>
@@ -5614,12 +5610,12 @@
         <v>1</v>
       </c>
       <c r="AH10" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="AI10" s="15">
-        <f t="shared" si="5"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="13"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AJ10" s="13" t="s">
         <v>62</v>
@@ -5631,12 +5627,12 @@
         <v>1</v>
       </c>
       <c r="AM10" s="14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="AN10" s="15">
-        <f t="shared" si="6"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="15"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AO10" s="13" t="s">
         <v>62</v>
@@ -5648,12 +5644,12 @@
         <v>1</v>
       </c>
       <c r="AR10" s="14">
-        <f t="shared" si="22"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AS10" s="15">
-        <f t="shared" si="7"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="17"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AT10" s="13" t="s">
         <v>62</v>
@@ -5665,12 +5661,12 @@
         <v>1</v>
       </c>
       <c r="AW10" s="14">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="AX10" s="15">
-        <f t="shared" si="8"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="19"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="AY10" s="13" t="s">
         <v>62</v>
@@ -5682,12 +5678,12 @@
         <v>1</v>
       </c>
       <c r="BB10" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="BC10" s="15">
-        <f t="shared" si="9"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="21"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BD10" s="13" t="s">
         <v>62</v>
@@ -5699,12 +5695,12 @@
         <v>1</v>
       </c>
       <c r="BG10" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="BH10" s="15">
-        <f t="shared" si="10"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="23"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BI10" s="13" t="s">
         <v>62</v>
@@ -5716,12 +5712,12 @@
         <v>1</v>
       </c>
       <c r="BL10" s="14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
       <c r="BM10" s="15">
-        <f t="shared" si="11"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="25"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BN10" s="13" t="s">
         <v>62</v>
@@ -5733,12 +5729,12 @@
         <v>1</v>
       </c>
       <c r="BQ10" s="14">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="BR10" s="15">
         <f t="shared" si="27"/>
-        <v>2</v>
-      </c>
-      <c r="BR10" s="15">
-        <f t="shared" si="12"/>
-        <v>0.133333333333333</v>
+        <v>0.153846153846154</v>
       </c>
       <c r="BS10" s="13" t="s">
         <v>62</v>
@@ -5754,8 +5750,8 @@
         <v>2</v>
       </c>
       <c r="BW10" s="15">
-        <f t="shared" si="13"/>
-        <v>0.133333333333333</v>
+        <f t="shared" si="29"/>
+        <v>0.153846153846154</v>
       </c>
       <c r="BX10" s="13"/>
       <c r="BY10" s="13">
@@ -5766,899 +5762,644 @@
       </c>
     </row>
     <row r="11" spans="1:78">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="17">
+        <f t="shared" ref="B11:I11" si="30">SUM(B5:B10)</f>
+        <v>6</v>
+      </c>
+      <c r="C11" s="17">
+        <f t="shared" si="30"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="17">
+        <f t="shared" si="30"/>
+        <v>13</v>
+      </c>
+      <c r="E11" s="15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="30"/>
+        <v>6</v>
+      </c>
+      <c r="H11" s="17">
+        <f t="shared" si="30"/>
+        <v>7</v>
+      </c>
+      <c r="I11" s="17">
+        <f t="shared" si="30"/>
+        <v>13</v>
+      </c>
+      <c r="J11" s="15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="L11" s="17">
+        <f>SUM(L5:L10)</f>
+        <v>6</v>
+      </c>
+      <c r="M11" s="17">
+        <f>SUM(M5:M10)</f>
+        <v>7</v>
+      </c>
+      <c r="N11" s="17">
+        <f>SUM(N5:N10)</f>
+        <v>13</v>
+      </c>
+      <c r="O11" s="15">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q11" s="17">
+        <f>SUM(Q5:Q10)</f>
+        <v>6</v>
+      </c>
+      <c r="R11" s="17">
+        <f>SUM(R5:R10)</f>
+        <v>7</v>
+      </c>
+      <c r="S11" s="17">
+        <f>SUM(S5:S10)</f>
+        <v>13</v>
+      </c>
+      <c r="T11" s="15">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="U11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="V11" s="17">
+        <f>SUM(V5:V10)</f>
+        <v>6</v>
+      </c>
+      <c r="W11" s="17">
+        <f>SUM(W5:W10)</f>
+        <v>7</v>
+      </c>
+      <c r="X11" s="17">
+        <f>SUM(X5:X10)</f>
+        <v>13</v>
+      </c>
+      <c r="Y11" s="15">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Z11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA11" s="17">
+        <f>SUM(AA5:AA10)</f>
+        <v>6</v>
+      </c>
+      <c r="AB11" s="17">
+        <f>SUM(AB5:AB10)</f>
+        <v>7</v>
+      </c>
+      <c r="AC11" s="17">
+        <f>SUM(AC5:AC10)</f>
+        <v>13</v>
+      </c>
+      <c r="AD11" s="15">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF11" s="17">
+        <f>SUM(AF5:AF10)</f>
+        <v>6</v>
+      </c>
+      <c r="AG11" s="17">
+        <f>SUM(AG5:AG10)</f>
+        <v>7</v>
+      </c>
+      <c r="AH11" s="17">
+        <f>SUM(AH5:AH10)</f>
+        <v>13</v>
+      </c>
+      <c r="AI11" s="15">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK11" s="17">
+        <f>SUM(AK5:AK10)</f>
+        <v>6</v>
+      </c>
+      <c r="AL11" s="17">
+        <f>SUM(AL5:AL10)</f>
+        <v>7</v>
+      </c>
+      <c r="AM11" s="17">
+        <f>SUM(AM5:AM10)</f>
+        <v>13</v>
+      </c>
+      <c r="AN11" s="15">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="AO11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP11" s="17">
+        <f>SUM(AP5:AP10)</f>
+        <v>6</v>
+      </c>
+      <c r="AQ11" s="17">
+        <f>SUM(AQ5:AQ10)</f>
+        <v>7</v>
+      </c>
+      <c r="AR11" s="17">
+        <f>SUM(AR5:AR10)</f>
+        <v>13</v>
+      </c>
+      <c r="AS11" s="15">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="AT11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AU11" s="17">
+        <f>SUM(AU5:AU10)</f>
+        <v>6</v>
+      </c>
+      <c r="AV11" s="17">
+        <f>SUM(AV5:AV10)</f>
+        <v>7</v>
+      </c>
+      <c r="AW11" s="17">
+        <f>SUM(AW5:AW10)</f>
+        <v>13</v>
+      </c>
+      <c r="AX11" s="15">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AY11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ11" s="17">
+        <f>SUM(AZ5:AZ10)</f>
+        <v>6</v>
+      </c>
+      <c r="BA11" s="17">
+        <f>SUM(BA5:BA10)</f>
+        <v>7</v>
+      </c>
+      <c r="BB11" s="17">
+        <f>SUM(BB5:BB10)</f>
+        <v>13</v>
+      </c>
+      <c r="BC11" s="15">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="BD11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE11" s="17">
+        <f>SUM(BE5:BE10)</f>
+        <v>6</v>
+      </c>
+      <c r="BF11" s="17">
+        <f>SUM(BF5:BF10)</f>
+        <v>7</v>
+      </c>
+      <c r="BG11" s="17">
+        <f>SUM(BG5:BG10)</f>
+        <v>13</v>
+      </c>
+      <c r="BH11" s="15">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="BI11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ11" s="17">
+        <f>SUM(BJ5:BJ10)</f>
+        <v>6</v>
+      </c>
+      <c r="BK11" s="17">
+        <f>SUM(BK5:BK10)</f>
+        <v>7</v>
+      </c>
+      <c r="BL11" s="17">
+        <f>SUM(BL5:BL10)</f>
+        <v>13</v>
+      </c>
+      <c r="BM11" s="15">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="BN11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="BO11" s="17">
+        <f>SUM(BO5:BO10)</f>
+        <v>6</v>
+      </c>
+      <c r="BP11" s="17">
+        <f>SUM(BP5:BP10)</f>
+        <v>7</v>
+      </c>
+      <c r="BQ11" s="17">
+        <f>SUM(BQ5:BQ10)</f>
+        <v>13</v>
+      </c>
+      <c r="BR11" s="15">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="BS11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="BT11" s="17">
+        <f>SUM(BT5:BT10)</f>
+        <v>6</v>
+      </c>
+      <c r="BU11" s="17">
+        <f>SUM(BU5:BU10)</f>
+        <v>7</v>
+      </c>
+      <c r="BV11" s="17">
+        <f>SUM(BV5:BV10)</f>
+        <v>13</v>
+      </c>
+      <c r="BW11" s="15">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="BX11" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="BY11" s="17">
+        <f>SUM(BY5:BY10)</f>
+        <v>6</v>
+      </c>
+      <c r="BZ11" s="17">
+        <f>SUM(BZ5:BZ10)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:73">
+      <c r="B12" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="13">
-        <v>1</v>
-      </c>
-      <c r="C11" s="13">
-        <v>1</v>
-      </c>
-      <c r="D11" s="14">
-        <f t="shared" si="14"/>
-        <v>2</v>
-      </c>
-      <c r="E11" s="15">
-        <f>D11/D$12</f>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="F11" s="13" t="s">
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="13">
-        <v>1</v>
-      </c>
-      <c r="H11" s="13">
-        <v>1</v>
-      </c>
-      <c r="I11" s="14">
-        <f t="shared" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="J11" s="15">
-        <f t="shared" si="0"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="K11" s="13" t="s">
+      <c r="H12" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" t="s">
         <v>63</v>
       </c>
-      <c r="L11" s="13">
-        <v>1</v>
-      </c>
-      <c r="M11" s="13">
-        <v>1</v>
-      </c>
-      <c r="N11" s="14">
-        <f t="shared" si="16"/>
-        <v>2</v>
-      </c>
-      <c r="O11" s="15">
-        <f t="shared" si="1"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="P11" s="13" t="s">
+      <c r="M12" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q12" t="s">
         <v>63</v>
       </c>
-      <c r="Q11" s="13">
-        <v>1</v>
-      </c>
-      <c r="R11" s="13">
-        <v>1</v>
-      </c>
-      <c r="S11" s="14">
-        <f t="shared" si="17"/>
-        <v>2</v>
-      </c>
-      <c r="T11" s="15">
-        <f t="shared" si="2"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="U11" s="13" t="s">
+      <c r="R12" t="s">
+        <v>64</v>
+      </c>
+      <c r="V12" t="s">
         <v>63</v>
       </c>
-      <c r="V11" s="13">
-        <v>1</v>
-      </c>
-      <c r="W11" s="13">
-        <v>1</v>
-      </c>
-      <c r="X11" s="14">
-        <f t="shared" si="18"/>
-        <v>2</v>
-      </c>
-      <c r="Y11" s="15">
-        <f t="shared" si="3"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="Z11" s="13" t="s">
+      <c r="W12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA12" t="s">
         <v>63</v>
       </c>
-      <c r="AA11" s="13">
-        <v>1</v>
-      </c>
-      <c r="AB11" s="13">
-        <v>1</v>
-      </c>
-      <c r="AC11" s="14">
-        <f t="shared" si="19"/>
-        <v>2</v>
-      </c>
-      <c r="AD11" s="15">
-        <f t="shared" si="4"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="AE11" s="13" t="s">
+      <c r="AB12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF12" t="s">
         <v>63</v>
       </c>
-      <c r="AF11" s="13">
-        <v>1</v>
-      </c>
-      <c r="AG11" s="13">
-        <v>1</v>
-      </c>
-      <c r="AH11" s="14">
-        <f t="shared" si="20"/>
-        <v>2</v>
-      </c>
-      <c r="AI11" s="15">
-        <f t="shared" si="5"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="AJ11" s="13" t="s">
+      <c r="AG12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK12" t="s">
         <v>63</v>
       </c>
-      <c r="AK11" s="13">
-        <v>1</v>
-      </c>
-      <c r="AL11" s="13">
-        <v>1</v>
-      </c>
-      <c r="AM11" s="14">
-        <f t="shared" si="21"/>
-        <v>2</v>
-      </c>
-      <c r="AN11" s="15">
-        <f t="shared" si="6"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="AO11" s="13" t="s">
+      <c r="AL12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AP12" t="s">
         <v>63</v>
       </c>
-      <c r="AP11" s="13">
-        <v>1</v>
-      </c>
-      <c r="AQ11" s="13">
-        <v>1</v>
-      </c>
-      <c r="AR11" s="14">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="AS11" s="15">
-        <f t="shared" si="7"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="AT11" s="13" t="s">
+      <c r="AQ12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AU12" t="s">
         <v>63</v>
       </c>
-      <c r="AU11" s="13">
-        <v>1</v>
-      </c>
-      <c r="AV11" s="13">
-        <v>1</v>
-      </c>
-      <c r="AW11" s="14">
-        <f t="shared" si="23"/>
-        <v>2</v>
-      </c>
-      <c r="AX11" s="15">
-        <f t="shared" si="8"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="AY11" s="13" t="s">
+      <c r="AV12" t="s">
+        <v>64</v>
+      </c>
+      <c r="AZ12" t="s">
         <v>63</v>
       </c>
-      <c r="AZ11" s="13">
-        <v>1</v>
-      </c>
-      <c r="BA11" s="13">
-        <v>1</v>
-      </c>
-      <c r="BB11" s="14">
-        <f t="shared" si="24"/>
-        <v>2</v>
-      </c>
-      <c r="BC11" s="15">
-        <f t="shared" si="9"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="BD11" s="13" t="s">
+      <c r="BA12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BE12" t="s">
         <v>63</v>
       </c>
-      <c r="BE11" s="13">
-        <v>1</v>
-      </c>
-      <c r="BF11" s="13">
-        <v>1</v>
-      </c>
-      <c r="BG11" s="14">
-        <f t="shared" si="25"/>
-        <v>2</v>
-      </c>
-      <c r="BH11" s="15">
-        <f t="shared" si="10"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="BI11" s="13" t="s">
+      <c r="BF12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BJ12" t="s">
         <v>63</v>
       </c>
-      <c r="BJ11" s="13">
-        <v>1</v>
-      </c>
-      <c r="BK11" s="13">
-        <v>1</v>
-      </c>
-      <c r="BL11" s="14">
-        <f t="shared" si="26"/>
-        <v>2</v>
-      </c>
-      <c r="BM11" s="15">
-        <f t="shared" si="11"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="BN11" s="13" t="s">
+      <c r="BK12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BO12" t="s">
         <v>63</v>
       </c>
-      <c r="BO11" s="13">
-        <v>1</v>
-      </c>
-      <c r="BP11" s="13">
-        <v>1</v>
-      </c>
-      <c r="BQ11" s="14">
-        <f t="shared" si="27"/>
-        <v>2</v>
-      </c>
-      <c r="BR11" s="15">
-        <f t="shared" si="12"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="BS11" s="13" t="s">
+      <c r="BP12" t="s">
+        <v>64</v>
+      </c>
+      <c r="BT12" t="s">
         <v>63</v>
       </c>
-      <c r="BT11" s="13">
-        <v>1</v>
-      </c>
-      <c r="BU11" s="13">
-        <v>1</v>
-      </c>
-      <c r="BV11" s="14">
-        <f t="shared" si="28"/>
-        <v>2</v>
-      </c>
-      <c r="BW11" s="15">
-        <f t="shared" si="13"/>
-        <v>0.133333333333333</v>
-      </c>
-      <c r="BX11" s="13"/>
-      <c r="BY11" s="13">
-        <v>1</v>
-      </c>
-      <c r="BZ11" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:78">
-      <c r="A12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="17">
-        <f t="shared" ref="B12:I12" si="29">SUM(B5:B11)</f>
-        <v>7</v>
-      </c>
-      <c r="C12" s="17">
-        <f t="shared" si="29"/>
-        <v>8</v>
-      </c>
-      <c r="D12" s="17">
-        <f t="shared" si="29"/>
-        <v>15</v>
-      </c>
-      <c r="E12" s="15">
-        <f>D12/D$12</f>
-        <v>1</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="17">
-        <f t="shared" si="29"/>
-        <v>7</v>
-      </c>
-      <c r="H12" s="17">
-        <f t="shared" si="29"/>
-        <v>8</v>
-      </c>
-      <c r="I12" s="17">
-        <f t="shared" si="29"/>
-        <v>15</v>
-      </c>
-      <c r="J12" s="15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="L12" s="17">
-        <f t="shared" ref="L12:N12" si="30">SUM(L5:L11)</f>
-        <v>7</v>
-      </c>
-      <c r="M12" s="17">
-        <f t="shared" si="30"/>
-        <v>8</v>
-      </c>
-      <c r="N12" s="17">
-        <f t="shared" si="30"/>
-        <v>15</v>
-      </c>
-      <c r="O12" s="15">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="P12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q12" s="17">
-        <f t="shared" ref="Q12:S12" si="31">SUM(Q5:Q11)</f>
-        <v>7</v>
-      </c>
-      <c r="R12" s="17">
-        <f t="shared" si="31"/>
-        <v>8</v>
-      </c>
-      <c r="S12" s="17">
-        <f t="shared" si="31"/>
-        <v>15</v>
-      </c>
-      <c r="T12" s="15">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="U12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="V12" s="17">
-        <f t="shared" ref="V12:X12" si="32">SUM(V5:V11)</f>
-        <v>7</v>
-      </c>
-      <c r="W12" s="17">
-        <f t="shared" si="32"/>
-        <v>8</v>
-      </c>
-      <c r="X12" s="17">
-        <f t="shared" si="32"/>
-        <v>15</v>
-      </c>
-      <c r="Y12" s="15">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="Z12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA12" s="17">
-        <f t="shared" ref="AA12:AC12" si="33">SUM(AA5:AA11)</f>
-        <v>7</v>
-      </c>
-      <c r="AB12" s="17">
-        <f t="shared" si="33"/>
-        <v>8</v>
-      </c>
-      <c r="AC12" s="17">
-        <f t="shared" si="33"/>
-        <v>15</v>
-      </c>
-      <c r="AD12" s="15">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="AE12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF12" s="17">
-        <f t="shared" ref="AF12:AH12" si="34">SUM(AF5:AF11)</f>
-        <v>7</v>
-      </c>
-      <c r="AG12" s="17">
-        <f t="shared" si="34"/>
-        <v>8</v>
-      </c>
-      <c r="AH12" s="17">
-        <f t="shared" si="34"/>
-        <v>15</v>
-      </c>
-      <c r="AI12" s="15">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="AJ12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="AK12" s="17">
-        <f t="shared" ref="AK12:AM12" si="35">SUM(AK5:AK11)</f>
-        <v>7</v>
-      </c>
-      <c r="AL12" s="17">
-        <f t="shared" si="35"/>
-        <v>8</v>
-      </c>
-      <c r="AM12" s="17">
-        <f t="shared" si="35"/>
-        <v>15</v>
-      </c>
-      <c r="AN12" s="15">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="AO12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="AP12" s="17">
-        <f t="shared" ref="AP12:AR12" si="36">SUM(AP5:AP11)</f>
-        <v>7</v>
-      </c>
-      <c r="AQ12" s="17">
-        <f t="shared" si="36"/>
-        <v>8</v>
-      </c>
-      <c r="AR12" s="17">
-        <f t="shared" si="36"/>
-        <v>15</v>
-      </c>
-      <c r="AS12" s="15">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="AT12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="AU12" s="17">
-        <f t="shared" ref="AU12:AW12" si="37">SUM(AU5:AU11)</f>
-        <v>7</v>
-      </c>
-      <c r="AV12" s="17">
-        <f t="shared" si="37"/>
-        <v>8</v>
-      </c>
-      <c r="AW12" s="17">
-        <f t="shared" si="37"/>
-        <v>15</v>
-      </c>
-      <c r="AX12" s="15">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="AY12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="AZ12" s="17">
-        <f t="shared" ref="AZ12:BB12" si="38">SUM(AZ5:AZ11)</f>
-        <v>7</v>
-      </c>
-      <c r="BA12" s="17">
-        <f t="shared" si="38"/>
-        <v>8</v>
-      </c>
-      <c r="BB12" s="17">
-        <f t="shared" si="38"/>
-        <v>15</v>
-      </c>
-      <c r="BC12" s="15">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="BD12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="BE12" s="17">
-        <f t="shared" ref="BE12:BG12" si="39">SUM(BE5:BE11)</f>
-        <v>7</v>
-      </c>
-      <c r="BF12" s="17">
-        <f t="shared" si="39"/>
-        <v>8</v>
-      </c>
-      <c r="BG12" s="17">
-        <f t="shared" si="39"/>
-        <v>15</v>
-      </c>
-      <c r="BH12" s="15">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="BI12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="BJ12" s="17">
-        <f t="shared" ref="BJ12:BL12" si="40">SUM(BJ5:BJ11)</f>
-        <v>7</v>
-      </c>
-      <c r="BK12" s="17">
-        <f t="shared" si="40"/>
-        <v>8</v>
-      </c>
-      <c r="BL12" s="17">
-        <f t="shared" si="40"/>
-        <v>15</v>
-      </c>
-      <c r="BM12" s="15">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="BN12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="BO12" s="17">
-        <f t="shared" ref="BO12:BQ12" si="41">SUM(BO5:BO11)</f>
-        <v>7</v>
-      </c>
-      <c r="BP12" s="17">
-        <f t="shared" si="41"/>
-        <v>8</v>
-      </c>
-      <c r="BQ12" s="17">
-        <f t="shared" si="41"/>
-        <v>15</v>
-      </c>
-      <c r="BR12" s="15">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="BS12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="BT12" s="17">
-        <f t="shared" ref="BT12:BV12" si="42">SUM(BT5:BT11)</f>
-        <v>7</v>
-      </c>
-      <c r="BU12" s="17">
-        <f t="shared" si="42"/>
-        <v>8</v>
-      </c>
-      <c r="BV12" s="17">
-        <f t="shared" si="42"/>
-        <v>15</v>
-      </c>
-      <c r="BW12" s="15">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="BX12" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="BY12" s="17">
-        <f>SUM(BY5:BY11)</f>
-        <v>7</v>
-      </c>
-      <c r="BZ12" s="17">
-        <f>SUM(BZ5:BZ11)</f>
-        <v>8</v>
+      <c r="BU12" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="2:73">
-      <c r="B13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13">
+        <f>B11/D11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="C13">
+        <f>C11/D11</f>
+        <v>0.538461538461538</v>
+      </c>
+      <c r="G13">
+        <f>G11/I11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="H13">
+        <f>H11/I11</f>
+        <v>0.538461538461538</v>
+      </c>
+      <c r="L13">
+        <f>L11/N11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="M13">
+        <f>M11/N11</f>
+        <v>0.538461538461538</v>
+      </c>
+      <c r="Q13">
+        <f>Q11/S11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="R13">
+        <f>R11/S11</f>
+        <v>0.538461538461538</v>
+      </c>
+      <c r="V13">
+        <f>V11/X11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="W13">
+        <f>W11/X11</f>
+        <v>0.538461538461538</v>
+      </c>
+      <c r="AA13">
+        <f>AA11/AC11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="AB13">
+        <f>AB11/AC11</f>
+        <v>0.538461538461538</v>
+      </c>
+      <c r="AF13">
+        <f>AF11/AH11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="AG13">
+        <f>AG11/AH11</f>
+        <v>0.538461538461538</v>
+      </c>
+      <c r="AK13">
+        <f>AK11/AM11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="AL13">
+        <f>AL11/AM11</f>
+        <v>0.538461538461538</v>
+      </c>
+      <c r="AP13">
+        <f>AP11/AR11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="AQ13">
+        <f>AQ11/AR11</f>
+        <v>0.538461538461538</v>
+      </c>
+      <c r="AU13">
+        <f>AU11/AW11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="AV13">
+        <f>AV11/AW11</f>
+        <v>0.538461538461538</v>
+      </c>
+      <c r="AZ13">
+        <f>AZ11/BB11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="BA13">
+        <f>BA11/BB11</f>
+        <v>0.538461538461538</v>
+      </c>
+      <c r="BE13">
+        <f>BE11/BG11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="BF13">
+        <f>BF11/BG11</f>
+        <v>0.538461538461538</v>
+      </c>
+      <c r="BJ13">
+        <f>BJ11/BL11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="BK13">
+        <f>BK11/BL11</f>
+        <v>0.538461538461538</v>
+      </c>
+      <c r="BO13">
+        <f>BO11/BQ11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="BP13">
+        <f>BP11/BQ11</f>
+        <v>0.538461538461538</v>
+      </c>
+      <c r="BT13">
+        <f>BT11/BV11</f>
+        <v>0.461538461538462</v>
+      </c>
+      <c r="BU13">
+        <f>BU11/BV11</f>
+        <v>0.538461538461538</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" spans="1:16">
+      <c r="A16" t="s">
         <v>65</v>
       </c>
-      <c r="G13" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" t="s">
-        <v>65</v>
-      </c>
-      <c r="L13" t="s">
-        <v>64</v>
-      </c>
-      <c r="M13" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>64</v>
-      </c>
-      <c r="R13" t="s">
-        <v>65</v>
-      </c>
-      <c r="V13" t="s">
-        <v>64</v>
-      </c>
-      <c r="W13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AK13" t="s">
-        <v>64</v>
-      </c>
-      <c r="AL13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AP13" t="s">
-        <v>64</v>
-      </c>
-      <c r="AQ13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AU13" t="s">
-        <v>64</v>
-      </c>
-      <c r="AV13" t="s">
-        <v>65</v>
-      </c>
-      <c r="AZ13" t="s">
-        <v>64</v>
-      </c>
-      <c r="BA13" t="s">
-        <v>65</v>
-      </c>
-      <c r="BE13" t="s">
-        <v>64</v>
-      </c>
-      <c r="BF13" t="s">
-        <v>65</v>
-      </c>
-      <c r="BJ13" t="s">
-        <v>64</v>
-      </c>
-      <c r="BK13" t="s">
-        <v>65</v>
-      </c>
-      <c r="BO13" t="s">
-        <v>64</v>
-      </c>
-      <c r="BP13" t="s">
-        <v>65</v>
-      </c>
-      <c r="BT13" t="s">
-        <v>64</v>
-      </c>
-      <c r="BU13" t="s">
-        <v>65</v>
-      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
     </row>
-    <row r="14" spans="2:73">
-      <c r="B14">
-        <f>B12/D12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="C14">
-        <f>C12/D12</f>
-        <v>0.533333333333333</v>
-      </c>
-      <c r="G14">
-        <f>G12/I12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="H14">
-        <f>H12/I12</f>
-        <v>0.533333333333333</v>
-      </c>
-      <c r="L14">
-        <f>L12/N12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="M14">
-        <f>M12/N12</f>
-        <v>0.533333333333333</v>
-      </c>
-      <c r="Q14">
-        <f>Q12/S12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="R14">
-        <f>R12/S12</f>
-        <v>0.533333333333333</v>
-      </c>
-      <c r="V14">
-        <f>V12/X12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="W14">
-        <f>W12/X12</f>
-        <v>0.533333333333333</v>
-      </c>
-      <c r="AA14">
-        <f>AA12/AC12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="AB14">
-        <f>AB12/AC12</f>
-        <v>0.533333333333333</v>
-      </c>
-      <c r="AF14">
-        <f>AF12/AH12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="AG14">
-        <f>AG12/AH12</f>
-        <v>0.533333333333333</v>
-      </c>
-      <c r="AK14">
-        <f>AK12/AM12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="AL14">
-        <f>AL12/AM12</f>
-        <v>0.533333333333333</v>
-      </c>
-      <c r="AP14">
-        <f>AP12/AR12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="AQ14">
-        <f>AQ12/AR12</f>
-        <v>0.533333333333333</v>
-      </c>
-      <c r="AU14">
-        <f>AU12/AW12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="AV14">
-        <f>AV12/AW12</f>
-        <v>0.533333333333333</v>
-      </c>
-      <c r="AZ14">
-        <f>AZ12/BB12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="BA14">
-        <f>BA12/BB12</f>
-        <v>0.533333333333333</v>
-      </c>
-      <c r="BE14">
-        <f>BE12/BG12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="BF14">
-        <f>BF12/BG12</f>
-        <v>0.533333333333333</v>
-      </c>
-      <c r="BJ14">
-        <f>BJ12/BL12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="BK14">
-        <f>BK12/BL12</f>
-        <v>0.533333333333333</v>
-      </c>
-      <c r="BO14">
-        <f>BO12/BQ12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="BP14">
-        <f>BP12/BQ12</f>
-        <v>0.533333333333333</v>
-      </c>
-      <c r="BT14">
-        <f>BT12/BV12</f>
-        <v>0.466666666666667</v>
-      </c>
-      <c r="BU14">
-        <f>BU12/BV12</f>
-        <v>0.533333333333333</v>
+    <row r="17" ht="76.55" spans="2:16">
+      <c r="B17" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="M17" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="N17" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="O17" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="P17" s="25" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="17" ht="14.25" spans="1:16">
-      <c r="A17" t="s">
+    <row r="18" spans="1:17">
+      <c r="A18" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19"/>
-      <c r="O17" s="19"/>
-      <c r="P17" s="19"/>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K18" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" t="s">
+        <v>41</v>
+      </c>
+      <c r="M18" t="s">
+        <v>42</v>
+      </c>
+      <c r="N18" t="s">
+        <v>42</v>
+      </c>
+      <c r="O18" t="s">
+        <v>42</v>
+      </c>
+      <c r="P18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="18" ht="76.55" spans="2:16">
-      <c r="B18" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="K18" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="L18" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="M18" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="N18" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="O18" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="P18" s="25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" t="s">
-        <v>41</v>
-      </c>
-      <c r="H19" t="s">
-        <v>41</v>
-      </c>
-      <c r="I19" t="s">
-        <v>41</v>
-      </c>
-      <c r="J19" t="s">
-        <v>41</v>
-      </c>
-      <c r="K19" t="s">
-        <v>42</v>
-      </c>
-      <c r="L19" t="s">
-        <v>41</v>
-      </c>
-      <c r="M19" t="s">
-        <v>42</v>
-      </c>
-      <c r="N19" t="s">
-        <v>42</v>
-      </c>
-      <c r="O19" t="s">
-        <v>42</v>
-      </c>
-      <c r="P19" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q19" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" s="23" t="s">
         <v>68</v>
+      </c>
+      <c r="B20">
+        <f>((C6/C11)*(H6/H11)*(M7/M11)*(R8/R11)*(W7/W11)*(AB7/AB11)*(AG7/AG11)*(AL7/AL11)*(AQ7/AQ11)*(AV8/AV11)*(BA7/BA11)*(BF8/BF11)*(BK8/BK11)*(BP8/BP11)*(BU8/BU11))</f>
+        <v>6.90206960591721e-9</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -6666,17 +6407,8 @@
         <v>69</v>
       </c>
       <c r="B21">
-        <f>((C6/C12)*(H6/H12)*(M7/M12)*(R8/R12)*(W7/W12)*(AB7/AB12)*(AG7/AG12)*(AL7/AL12)*(AQ7/AQ12)*(AV8/AV12)*(BA7/BA12)*(BF8/BF12)*(BK8/BK12)*(BP8/BP12)*(BU8/BU12))</f>
-        <v>9.31322574615479e-10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22">
-        <f>((B6/B12)*(G6/G12)*(L7/L12)*(Q8/Q12)*(V7/V12)*(AA7/AA12)*(AF7/AF12)*(AK7/AK12)*(AP7/AP12)*(AU8/AU12)*(AZ7/AZ12)*(BE8/BE12)*(BJ8/BJ12)*(BO8/BO12)*(BT8/BT12))</f>
-        <v>2.10634448422766e-13</v>
+        <f>((B6/B11)*(G6/G11)*(L7/L11)*(Q8/Q11)*(V7/V11)*(AA7/AA11)*(AF7/AF11)*(AK7/AK11)*(AP7/AP11)*(AU8/AU11)*(AZ7/AZ11)*(BE8/BE11)*(BJ8/BJ11)*(BO8/BO11)*(BT8/BT11))</f>
+        <v>2.12682249073048e-12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: NaiveBayesV3Controller.naiveBayesClassifier (beta concept)
</commit_message>
<xml_diff>
--- a/hitung_manual.xlsx
+++ b/hitung_manual.xlsx
@@ -2918,8 +2918,8 @@
   <sheetPr/>
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="5"/>
@@ -3793,8 +3793,8 @@
   <sheetPr/>
   <dimension ref="A1:BZ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:M18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -6348,7 +6348,7 @@
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
         <v>41</v>
@@ -6398,8 +6398,8 @@
         <v>68</v>
       </c>
       <c r="B20">
-        <f>((C6/C11)*(H6/H11)*(M7/M11)*(R8/R11)*(W7/W11)*(AB7/AB11)*(AG7/AG11)*(AL7/AL11)*(AQ7/AQ11)*(AV8/AV11)*(BA7/BA11)*(BF8/BF11)*(BK8/BK11)*(BP8/BP11)*(BU8/BU11))</f>
-        <v>6.90206960591721e-9</v>
+        <f>((C6/C11)*(H7/H11)*(M7/M11)*(R8/R11)*(W7/W11)*(AB7/AB11)*(AG7/AG11)*(AL7/AL11)*(AQ7/AQ11)*(AV8/AV11)*(BA7/BA11)*(BF8/BF11)*(BK8/BK11)*(BP8/BP11)*(BU8/BU11))</f>
+        <v>3.4510348029586e-9</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -6407,7 +6407,7 @@
         <v>69</v>
       </c>
       <c r="B21">
-        <f>((B6/B11)*(G6/G11)*(L7/L11)*(Q8/Q11)*(V7/V11)*(AA7/AA11)*(AF7/AF11)*(AK7/AK11)*(AP7/AP11)*(AU8/AU11)*(AZ7/AZ11)*(BE8/BE11)*(BJ8/BJ11)*(BO8/BO11)*(BT8/BT11))</f>
+        <f>((B6/B11)*(G7/G11)*(L7/L11)*(Q8/Q11)*(V7/V11)*(AA7/AA11)*(AF7/AF11)*(AK7/AK11)*(AP7/AP11)*(AU8/AU11)*(AZ7/AZ11)*(BE8/BE11)*(BJ8/BJ11)*(BO8/BO11)*(BT8/BT11))</f>
         <v>2.12682249073048e-12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update: createTrainingData (fix empty array problem)
</commit_message>
<xml_diff>
--- a/hitung_manual.xlsx
+++ b/hitung_manual.xlsx
@@ -3375,7 +3375,7 @@
   <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -3453,7 +3453,7 @@
         <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
         <v>41</v>
@@ -3793,8 +3793,8 @@
   <sheetPr/>
   <dimension ref="A1:BZ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -4466,15 +4466,15 @@
         <v>1</v>
       </c>
       <c r="H6" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="14">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J6" s="15">
         <f t="shared" si="3"/>
-        <v>0.230769230769231</v>
+        <v>0.153846153846154</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>40</v>
@@ -4730,15 +4730,15 @@
         <v>1</v>
       </c>
       <c r="H7" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" s="14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J7" s="15">
         <f t="shared" si="3"/>
-        <v>0.153846153846154</v>
+        <v>0.230769230769231</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>41</v>
@@ -6399,7 +6399,7 @@
       </c>
       <c r="B20">
         <f>((C6/C11)*(H7/H11)*(M7/M11)*(R8/R11)*(W7/W11)*(AB7/AB11)*(AG7/AG11)*(AL7/AL11)*(AQ7/AQ11)*(AV8/AV11)*(BA7/BA11)*(BF8/BF11)*(BK8/BK11)*(BP8/BP11)*(BU8/BU11))</f>
-        <v>3.4510348029586e-9</v>
+        <v>6.90206960591721e-9</v>
       </c>
     </row>
     <row r="21" spans="1:2">

</xml_diff>